<commit_message>
Added more testdata + fixed selection bug + added comments for AdminController
</commit_message>
<xml_diff>
--- a/TESTDATA/test.xlsx
+++ b/TESTDATA/test.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Private\Repos\ProjectArla\TESTDATA\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{542C370A-4B8F-4C1C-AF9D-1428D632B0E5}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ED66A488-2ACC-4585-9FAA-231512F034B8}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28005" yWindow="8265" windowWidth="28470" windowHeight="15555" xr2:uid="{B22FC46E-052D-4056-BDC8-2AAC2DF1C145}"/>
+    <workbookView xWindow="8130" yWindow="5490" windowWidth="28470" windowHeight="15555" xr2:uid="{B22FC46E-052D-4056-BDC8-2AAC2DF1C145}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -39,10 +39,10 @@
     <t>Year</t>
   </si>
   <si>
-    <t>Header1</t>
+    <t>Creamy White</t>
   </si>
   <si>
-    <t>Header2</t>
+    <t>Creamy Blue</t>
   </si>
 </sst>
 </file>
@@ -397,7 +397,7 @@
   <dimension ref="A1:C5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+      <selection activeCell="D1" sqref="D1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -415,46 +415,46 @@
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2">
-        <v>2012</v>
+        <v>2016</v>
       </c>
       <c r="B2">
-        <v>50</v>
+        <v>30</v>
       </c>
       <c r="C2">
-        <v>30</v>
+        <v>47</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3">
-        <v>2013</v>
+        <v>2017</v>
       </c>
       <c r="B3">
-        <v>52</v>
+        <v>45</v>
       </c>
       <c r="C3">
-        <v>44</v>
+        <v>33</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4">
-        <v>2014</v>
+        <v>2018</v>
       </c>
       <c r="B4">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="C4">
-        <v>45</v>
+        <v>66</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5">
-        <v>2015</v>
+        <v>2019</v>
       </c>
       <c r="B5">
-        <v>10</v>
+        <v>23</v>
       </c>
       <c r="C5">
-        <v>10</v>
+        <v>78</v>
       </c>
     </row>
   </sheetData>

</xml_diff>